<commit_message>
Identity and report fix
</commit_message>
<xml_diff>
--- a/wwwroot/Reports/comments_report.xlsx
+++ b/wwwroot/Reports/comments_report.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Отчёт по комментариям</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>Atom - мой выбор для редактирования кода - он просто отличный!</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1371,6 +1374,17 @@
         <v>73</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" s="0">
+        <v>70</v>
+      </c>
+      <c r="B72" s="0">
+        <v>76</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:D1"/>

</xml_diff>